<commit_message>
Added column names and updated individual datasets
</commit_message>
<xml_diff>
--- a/datasets/monthly_gdp.xlsx
+++ b/datasets/monthly_gdp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Users\Kathleen\Monthly GDP\monthly gdp for website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ali_ahad/Desktop/rmsc4002/part2/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E540AD7B-8C2C-416C-8605-48A0BEBD5982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E4BCE9-0E43-A548-B072-423EE7DF50DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="22" r:id="rId1"/>
@@ -1204,7 +1204,7 @@
     <numFmt numFmtId="167" formatCode="\ [$-409]d\ mmmm\ yyyy"/>
     <numFmt numFmtId="168" formatCode="dd\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1820,7 +1820,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2616,7 +2616,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2963,7 +2963,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3310,7 +3310,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3957,7 +3957,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10047,31 +10047,31 @@
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="2.875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="11.875" style="9" customWidth="1"/>
-    <col min="3" max="16384" width="9.625" style="9"/>
+    <col min="1" max="1" width="2.83203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="9.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="7" customFormat="1" ht="20" customHeight="1">
       <c r="L1" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="25">
       <c r="B3" s="10" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="20.25" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="53">
         <v>44137</v>
       </c>
       <c r="C4" s="53"/>
     </row>
-    <row r="5" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="12.75" customHeight="1">
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51"/>
@@ -10080,51 +10080,51 @@
       <c r="G5" s="52"/>
       <c r="H5" s="51"/>
     </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="14" customFormat="1" ht="14">
       <c r="A6" s="12"/>
       <c r="B6" s="18" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="14" customFormat="1" ht="14">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="14" customFormat="1">
       <c r="A8" s="12"/>
       <c r="B8" s="13"/>
     </row>
-    <row r="9" spans="1:12" s="15" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="15" customFormat="1" ht="95.25" customHeight="1"/>
+    <row r="15" spans="1:12">
       <c r="E15" s="16"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" s="17"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4">
       <c r="B21" s="17"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4">
       <c r="B22" s="17"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4">
       <c r="B23" s="17"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4">
       <c r="B24" s="17"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4">
       <c r="B25" s="17"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4">
       <c r="B26" s="17"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4">
       <c r="B27" s="17"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4">
       <c r="D29" s="9" t="s">
         <v>344</v>
       </c>
@@ -10154,24 +10154,24 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="3.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="18.25" style="25" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="25" hidden="1" customWidth="1"/>
-    <col min="4" max="15" width="6.375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" style="25" hidden="1" customWidth="1"/>
+    <col min="4" max="15" width="6.33203125" style="25" customWidth="1"/>
     <col min="16" max="16384" width="8" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:15" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:15" ht="5.25" customHeight="1"/>
+    <row r="2" spans="2:15" ht="35" customHeight="1">
       <c r="B2" s="39" t="s">
         <v>320</v>
       </c>
       <c r="H2" s="34"/>
       <c r="O2" s="33"/>
     </row>
-    <row r="3" spans="2:15" ht="2.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:15" ht="2" customHeight="1">
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
       <c r="G3" s="44"/>
@@ -10180,7 +10180,7 @@
       <c r="J3" s="45"/>
       <c r="O3"/>
     </row>
-    <row r="4" spans="2:15" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:15" s="27" customFormat="1" ht="15" customHeight="1">
       <c r="B4" s="56">
         <v>44137</v>
       </c>
@@ -10198,8 +10198,8 @@
       <c r="N4" s="56"/>
       <c r="O4" s="56"/>
     </row>
-    <row r="5" spans="2:15" ht="2.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="2:15" ht="3.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:15" ht="2" customHeight="1"/>
+    <row r="6" spans="2:15" ht="3.75" customHeight="1">
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
       <c r="E6" s="46"/>
@@ -10212,7 +10212,7 @@
       <c r="N6" s="49"/>
       <c r="O6" s="49"/>
     </row>
-    <row r="7" spans="2:15" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:15" ht="1.5" customHeight="1">
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
@@ -10228,7 +10228,7 @@
       <c r="N7" s="24"/>
       <c r="O7" s="24"/>
     </row>
-    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:15" ht="14.25" customHeight="1">
       <c r="B8" s="37"/>
       <c r="C8" s="32" t="s">
         <v>339</v>
@@ -10270,7 +10270,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:15" ht="14.25" customHeight="1">
       <c r="B9" s="50" t="s">
         <v>321</v>
       </c>
@@ -10314,7 +10314,7 @@
         <v>18734.979190790575</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:15" ht="14.25" customHeight="1">
       <c r="B10" s="42" t="s">
         <v>322</v>
       </c>
@@ -10356,7 +10356,7 @@
         <v>0.95273770017858528</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15" ht="14.25" customHeight="1">
       <c r="B11" s="42" t="s">
         <v>323</v>
       </c>
@@ -10397,7 +10397,7 @@
         <v>12.051380351448039</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15" ht="14" customHeight="1">
       <c r="B12" s="29"/>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
@@ -10412,7 +10412,7 @@
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
     </row>
-    <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:15" ht="15" customHeight="1">
       <c r="B13" s="54" t="s">
         <v>350</v>
       </c>
@@ -10432,7 +10432,7 @@
       <c r="N13" s="57"/>
       <c r="O13" s="57"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:15">
       <c r="B14" s="37"/>
       <c r="D14" s="35" t="s">
         <v>373</v>
@@ -10445,7 +10445,7 @@
       </c>
       <c r="G14" s="26"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15">
       <c r="B15" s="27" t="s">
         <v>351</v>
       </c>
@@ -10460,7 +10460,7 @@
       </c>
       <c r="G15" s="28"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:15">
       <c r="B16" s="27" t="s">
         <v>352</v>
       </c>
@@ -10475,7 +10475,7 @@
       </c>
       <c r="G16" s="28"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15">
       <c r="B17" s="27" t="s">
         <v>353</v>
       </c>
@@ -10490,7 +10490,7 @@
       </c>
       <c r="G17" s="28"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15">
       <c r="B18" s="27" t="s">
         <v>354</v>
       </c>
@@ -10505,7 +10505,7 @@
       </c>
       <c r="G18" s="28"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15">
       <c r="B19" s="27" t="s">
         <v>355</v>
       </c>
@@ -10520,7 +10520,7 @@
       </c>
       <c r="G19" s="28"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15">
       <c r="B20" s="27" t="s">
         <v>356</v>
       </c>
@@ -10535,7 +10535,7 @@
       </c>
       <c r="G20" s="28"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15">
       <c r="B21" s="27" t="s">
         <v>357</v>
       </c>
@@ -10550,7 +10550,7 @@
       </c>
       <c r="G21" s="28"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15">
       <c r="B22" s="27" t="s">
         <v>358</v>
       </c>
@@ -10565,7 +10565,7 @@
       </c>
       <c r="G22" s="28"/>
     </row>
-    <row r="23" spans="2:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" ht="14">
       <c r="B23" s="27" t="s">
         <v>359</v>
       </c>
@@ -10588,7 +10588,7 @@
       <c r="N23"/>
       <c r="O23"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15">
       <c r="B24" s="36" t="s">
         <v>360</v>
       </c>
@@ -10604,10 +10604,10 @@
       </c>
       <c r="G24" s="28"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15">
       <c r="B25" s="27"/>
     </row>
-    <row r="26" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" ht="15" customHeight="1">
       <c r="B26" s="54" t="s">
         <v>350</v>
       </c>
@@ -10616,98 +10616,98 @@
       <c r="E26" s="54"/>
       <c r="F26" s="54"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15">
       <c r="B27" s="21"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15">
       <c r="B28" s="55"/>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
       <c r="E28" s="55"/>
       <c r="F28" s="55"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15">
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15">
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15">
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15">
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:15">
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:15">
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:15">
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:15">
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:15">
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
       <c r="F37" s="20"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:15">
       <c r="B38" s="55"/>
       <c r="C38" s="55"/>
       <c r="D38" s="55"/>
       <c r="E38" s="55"/>
       <c r="F38" s="55"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:15">
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
       <c r="F39" s="20"/>
     </row>
-    <row r="40" spans="2:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:15" ht="14">
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
       <c r="D40" s="20"/>
@@ -10722,112 +10722,112 @@
       <c r="N40"/>
       <c r="O40"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:15">
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
       <c r="D41" s="20"/>
       <c r="E41" s="20"/>
       <c r="F41" s="20"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:15">
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
       <c r="F42" s="20"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:15">
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:15">
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
       <c r="F44" s="20"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:15">
       <c r="B45" s="20"/>
       <c r="C45" s="20"/>
       <c r="D45" s="20"/>
       <c r="E45" s="20"/>
       <c r="F45" s="20"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:15">
       <c r="B46" s="20"/>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
       <c r="F46" s="20"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:15">
       <c r="B47" s="55"/>
       <c r="C47" s="55"/>
       <c r="D47" s="55"/>
       <c r="E47" s="55"/>
       <c r="F47" s="55"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:15">
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
       <c r="D48" s="20"/>
       <c r="E48" s="20"/>
       <c r="F48" s="20"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:15">
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:15">
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:15">
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:15">
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
       <c r="F52" s="20"/>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:15">
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
       <c r="E53" s="20"/>
       <c r="F53" s="20"/>
     </row>
-    <row r="54" spans="2:15" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:15" ht="9.75" customHeight="1">
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
       <c r="D54" s="20"/>
       <c r="E54" s="20"/>
       <c r="F54" s="20"/>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:15">
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
       <c r="D55" s="20"/>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
     </row>
-    <row r="56" spans="2:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:15" ht="14">
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
@@ -10843,7 +10843,7 @@
       <c r="N56"/>
       <c r="O56"/>
     </row>
-    <row r="57" spans="2:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:15" ht="14">
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
@@ -10881,22 +10881,22 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H347"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B335" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C346" sqref="C346"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="10.375" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1"/>
-    <col min="5" max="6" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="5" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="28">
       <c r="A1" s="1"/>
       <c r="B1" s="19" t="s">
         <v>276</v>
@@ -10907,7 +10907,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>274</v>
       </c>
@@ -10921,7 +10921,7 @@
       <c r="F2" s="3"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>273</v>
       </c>
@@ -10935,7 +10935,7 @@
       <c r="F3" s="3"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>272</v>
       </c>
@@ -10949,7 +10949,7 @@
       <c r="F4" s="3"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>271</v>
       </c>
@@ -10964,7 +10964,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>270</v>
       </c>
@@ -10979,7 +10979,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>269</v>
       </c>
@@ -10994,7 +10994,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>268</v>
       </c>
@@ -11009,7 +11009,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>267</v>
       </c>
@@ -11024,7 +11024,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>266</v>
       </c>
@@ -11039,7 +11039,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>265</v>
       </c>
@@ -11054,7 +11054,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>264</v>
       </c>
@@ -11069,7 +11069,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>263</v>
       </c>
@@ -11084,7 +11084,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>262</v>
       </c>
@@ -11099,7 +11099,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>261</v>
       </c>
@@ -11114,7 +11114,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>260</v>
       </c>
@@ -11129,7 +11129,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>259</v>
       </c>
@@ -11144,7 +11144,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>258</v>
       </c>
@@ -11159,7 +11159,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>257</v>
       </c>
@@ -11174,7 +11174,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>256</v>
       </c>
@@ -11189,7 +11189,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>255</v>
       </c>
@@ -11204,7 +11204,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>254</v>
       </c>
@@ -11219,7 +11219,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>253</v>
       </c>
@@ -11235,7 +11235,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>252</v>
       </c>
@@ -11251,7 +11251,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>251</v>
       </c>
@@ -11267,7 +11267,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
         <v>250</v>
       </c>
@@ -11283,7 +11283,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>249</v>
       </c>
@@ -11299,7 +11299,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>248</v>
       </c>
@@ -11315,7 +11315,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>247</v>
       </c>
@@ -11331,7 +11331,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>246</v>
       </c>
@@ -11347,7 +11347,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>245</v>
       </c>
@@ -11363,7 +11363,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>244</v>
       </c>
@@ -11379,7 +11379,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>243</v>
       </c>
@@ -11395,7 +11395,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>242</v>
       </c>
@@ -11411,7 +11411,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>241</v>
       </c>
@@ -11427,7 +11427,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>240</v>
       </c>
@@ -11443,7 +11443,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>239</v>
       </c>
@@ -11459,7 +11459,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>238</v>
       </c>
@@ -11475,7 +11475,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>237</v>
       </c>
@@ -11491,7 +11491,7 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>236</v>
       </c>
@@ -11507,7 +11507,7 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>235</v>
       </c>
@@ -11523,7 +11523,7 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>234</v>
       </c>
@@ -11539,7 +11539,7 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>233</v>
       </c>
@@ -11555,7 +11555,7 @@
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>232</v>
       </c>
@@ -11571,7 +11571,7 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>231</v>
       </c>
@@ -11587,7 +11587,7 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>230</v>
       </c>
@@ -11603,7 +11603,7 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>229</v>
       </c>
@@ -11619,7 +11619,7 @@
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>228</v>
       </c>
@@ -11635,7 +11635,7 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>227</v>
       </c>
@@ -11651,7 +11651,7 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>226</v>
       </c>
@@ -11667,7 +11667,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>225</v>
       </c>
@@ -11683,7 +11683,7 @@
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>224</v>
       </c>
@@ -11699,7 +11699,7 @@
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>223</v>
       </c>
@@ -11715,7 +11715,7 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>222</v>
       </c>
@@ -11731,7 +11731,7 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
         <v>221</v>
       </c>
@@ -11747,7 +11747,7 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
         <v>220</v>
       </c>
@@ -11763,7 +11763,7 @@
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>219</v>
       </c>
@@ -11779,7 +11779,7 @@
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
         <v>218</v>
       </c>
@@ -11795,7 +11795,7 @@
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
         <v>217</v>
       </c>
@@ -11811,7 +11811,7 @@
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
         <v>216</v>
       </c>
@@ -11827,7 +11827,7 @@
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
         <v>215</v>
       </c>
@@ -11843,7 +11843,7 @@
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>214</v>
       </c>
@@ -11859,7 +11859,7 @@
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>213</v>
       </c>
@@ -11875,7 +11875,7 @@
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
         <v>212</v>
       </c>
@@ -11891,7 +11891,7 @@
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
         <v>211</v>
       </c>
@@ -11907,7 +11907,7 @@
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
         <v>210</v>
       </c>
@@ -11923,7 +11923,7 @@
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
         <v>209</v>
       </c>
@@ -11939,7 +11939,7 @@
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
         <v>208</v>
       </c>
@@ -11955,7 +11955,7 @@
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
         <v>207</v>
       </c>
@@ -11971,7 +11971,7 @@
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
         <v>206</v>
       </c>
@@ -11987,7 +11987,7 @@
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
         <v>205</v>
       </c>
@@ -12003,7 +12003,7 @@
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
         <v>204</v>
       </c>
@@ -12019,7 +12019,7 @@
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
         <v>203</v>
       </c>
@@ -12035,7 +12035,7 @@
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
         <v>202</v>
       </c>
@@ -12051,7 +12051,7 @@
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
         <v>201</v>
       </c>
@@ -12067,7 +12067,7 @@
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
         <v>200</v>
       </c>
@@ -12083,7 +12083,7 @@
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
         <v>199</v>
       </c>
@@ -12099,7 +12099,7 @@
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
         <v>198</v>
       </c>
@@ -12115,7 +12115,7 @@
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8">
       <c r="A79" s="1" t="s">
         <v>197</v>
       </c>
@@ -12131,7 +12131,7 @@
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8">
       <c r="A80" s="1" t="s">
         <v>196</v>
       </c>
@@ -12147,7 +12147,7 @@
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8">
       <c r="A81" s="1" t="s">
         <v>195</v>
       </c>
@@ -12163,7 +12163,7 @@
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8">
       <c r="A82" s="1" t="s">
         <v>194</v>
       </c>
@@ -12179,7 +12179,7 @@
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8">
       <c r="A83" s="1" t="s">
         <v>193</v>
       </c>
@@ -12195,7 +12195,7 @@
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8">
       <c r="A84" s="1" t="s">
         <v>192</v>
       </c>
@@ -12211,7 +12211,7 @@
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8">
       <c r="A85" s="1" t="s">
         <v>191</v>
       </c>
@@ -12227,7 +12227,7 @@
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8">
       <c r="A86" s="1" t="s">
         <v>190</v>
       </c>
@@ -12243,7 +12243,7 @@
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8">
       <c r="A87" s="1" t="s">
         <v>189</v>
       </c>
@@ -12259,7 +12259,7 @@
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8">
       <c r="A88" s="1" t="s">
         <v>188</v>
       </c>
@@ -12275,7 +12275,7 @@
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8">
       <c r="A89" s="1" t="s">
         <v>187</v>
       </c>
@@ -12291,7 +12291,7 @@
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8">
       <c r="A90" s="1" t="s">
         <v>186</v>
       </c>
@@ -12307,7 +12307,7 @@
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8">
       <c r="A91" s="1" t="s">
         <v>185</v>
       </c>
@@ -12323,7 +12323,7 @@
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8">
       <c r="A92" s="1" t="s">
         <v>184</v>
       </c>
@@ -12339,7 +12339,7 @@
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8">
       <c r="A93" s="1" t="s">
         <v>183</v>
       </c>
@@ -12355,7 +12355,7 @@
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8">
       <c r="A94" s="1" t="s">
         <v>182</v>
       </c>
@@ -12371,7 +12371,7 @@
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8">
       <c r="A95" s="1" t="s">
         <v>181</v>
       </c>
@@ -12387,7 +12387,7 @@
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8">
       <c r="A96" s="1" t="s">
         <v>180</v>
       </c>
@@ -12403,7 +12403,7 @@
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8">
       <c r="A97" s="1" t="s">
         <v>179</v>
       </c>
@@ -12419,7 +12419,7 @@
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8">
       <c r="A98" s="1" t="s">
         <v>178</v>
       </c>
@@ -12435,7 +12435,7 @@
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8">
       <c r="A99" s="1" t="s">
         <v>177</v>
       </c>
@@ -12451,7 +12451,7 @@
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8">
       <c r="A100" s="1" t="s">
         <v>176</v>
       </c>
@@ -12467,7 +12467,7 @@
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8">
       <c r="A101" s="1" t="s">
         <v>175</v>
       </c>
@@ -12483,7 +12483,7 @@
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8">
       <c r="A102" s="1" t="s">
         <v>174</v>
       </c>
@@ -12499,7 +12499,7 @@
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8">
       <c r="A103" s="1" t="s">
         <v>173</v>
       </c>
@@ -12515,7 +12515,7 @@
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8">
       <c r="A104" s="1" t="s">
         <v>172</v>
       </c>
@@ -12531,7 +12531,7 @@
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8">
       <c r="A105" s="1" t="s">
         <v>171</v>
       </c>
@@ -12547,7 +12547,7 @@
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8">
       <c r="A106" s="1" t="s">
         <v>170</v>
       </c>
@@ -12563,7 +12563,7 @@
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8">
       <c r="A107" s="1" t="s">
         <v>169</v>
       </c>
@@ -12579,7 +12579,7 @@
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8">
       <c r="A108" s="1" t="s">
         <v>168</v>
       </c>
@@ -12595,7 +12595,7 @@
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8">
       <c r="A109" s="1" t="s">
         <v>167</v>
       </c>
@@ -12611,7 +12611,7 @@
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8">
       <c r="A110" s="1" t="s">
         <v>166</v>
       </c>
@@ -12627,7 +12627,7 @@
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8">
       <c r="A111" s="1" t="s">
         <v>165</v>
       </c>
@@ -12643,7 +12643,7 @@
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8">
       <c r="A112" s="1" t="s">
         <v>164</v>
       </c>
@@ -12659,7 +12659,7 @@
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8">
       <c r="A113" s="1" t="s">
         <v>163</v>
       </c>
@@ -12675,7 +12675,7 @@
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8">
       <c r="A114" s="1" t="s">
         <v>162</v>
       </c>
@@ -12691,7 +12691,7 @@
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8">
       <c r="A115" s="1" t="s">
         <v>161</v>
       </c>
@@ -12707,7 +12707,7 @@
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8">
       <c r="A116" s="1" t="s">
         <v>160</v>
       </c>
@@ -12723,7 +12723,7 @@
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8">
       <c r="A117" s="1" t="s">
         <v>159</v>
       </c>
@@ -12739,7 +12739,7 @@
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8">
       <c r="A118" s="1" t="s">
         <v>158</v>
       </c>
@@ -12755,7 +12755,7 @@
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8">
       <c r="A119" s="1" t="s">
         <v>157</v>
       </c>
@@ -12771,7 +12771,7 @@
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8">
       <c r="A120" s="1" t="s">
         <v>156</v>
       </c>
@@ -12787,7 +12787,7 @@
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8">
       <c r="A121" s="1" t="s">
         <v>155</v>
       </c>
@@ -12803,7 +12803,7 @@
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8">
       <c r="A122" s="1" t="s">
         <v>154</v>
       </c>
@@ -12819,7 +12819,7 @@
       <c r="G122" s="4"/>
       <c r="H122" s="4"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8">
       <c r="A123" s="1" t="s">
         <v>153</v>
       </c>
@@ -12835,7 +12835,7 @@
       <c r="G123" s="4"/>
       <c r="H123" s="4"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8">
       <c r="A124" s="1" t="s">
         <v>152</v>
       </c>
@@ -12851,7 +12851,7 @@
       <c r="G124" s="4"/>
       <c r="H124" s="4"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8">
       <c r="A125" s="1" t="s">
         <v>151</v>
       </c>
@@ -12867,7 +12867,7 @@
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8">
       <c r="A126" s="1" t="s">
         <v>150</v>
       </c>
@@ -12883,7 +12883,7 @@
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8">
       <c r="A127" s="1" t="s">
         <v>149</v>
       </c>
@@ -12899,7 +12899,7 @@
       <c r="G127" s="4"/>
       <c r="H127" s="4"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8">
       <c r="A128" s="1" t="s">
         <v>148</v>
       </c>
@@ -12915,7 +12915,7 @@
       <c r="G128" s="4"/>
       <c r="H128" s="4"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8">
       <c r="A129" s="1" t="s">
         <v>147</v>
       </c>
@@ -12931,7 +12931,7 @@
       <c r="G129" s="4"/>
       <c r="H129" s="4"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8">
       <c r="A130" s="1" t="s">
         <v>146</v>
       </c>
@@ -12947,7 +12947,7 @@
       <c r="G130" s="4"/>
       <c r="H130" s="4"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8">
       <c r="A131" s="1" t="s">
         <v>145</v>
       </c>
@@ -12963,7 +12963,7 @@
       <c r="G131" s="4"/>
       <c r="H131" s="4"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8">
       <c r="A132" s="1" t="s">
         <v>144</v>
       </c>
@@ -12979,7 +12979,7 @@
       <c r="G132" s="4"/>
       <c r="H132" s="4"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8">
       <c r="A133" s="1" t="s">
         <v>143</v>
       </c>
@@ -12995,7 +12995,7 @@
       <c r="G133" s="4"/>
       <c r="H133" s="4"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8">
       <c r="A134" s="1" t="s">
         <v>142</v>
       </c>
@@ -13011,7 +13011,7 @@
       <c r="G134" s="4"/>
       <c r="H134" s="4"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8">
       <c r="A135" s="1" t="s">
         <v>141</v>
       </c>
@@ -13027,7 +13027,7 @@
       <c r="G135" s="4"/>
       <c r="H135" s="4"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8">
       <c r="A136" s="1" t="s">
         <v>140</v>
       </c>
@@ -13043,7 +13043,7 @@
       <c r="G136" s="4"/>
       <c r="H136" s="4"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8">
       <c r="A137" s="1" t="s">
         <v>139</v>
       </c>
@@ -13059,7 +13059,7 @@
       <c r="G137" s="4"/>
       <c r="H137" s="4"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8">
       <c r="A138" s="1" t="s">
         <v>138</v>
       </c>
@@ -13075,7 +13075,7 @@
       <c r="G138" s="4"/>
       <c r="H138" s="4"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8">
       <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
@@ -13091,7 +13091,7 @@
       <c r="G139" s="4"/>
       <c r="H139" s="4"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8">
       <c r="A140" s="1" t="s">
         <v>136</v>
       </c>
@@ -13107,7 +13107,7 @@
       <c r="G140" s="4"/>
       <c r="H140" s="4"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8">
       <c r="A141" s="1" t="s">
         <v>135</v>
       </c>
@@ -13123,7 +13123,7 @@
       <c r="G141" s="4"/>
       <c r="H141" s="4"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8">
       <c r="A142" s="1" t="s">
         <v>134</v>
       </c>
@@ -13139,7 +13139,7 @@
       <c r="G142" s="4"/>
       <c r="H142" s="4"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8">
       <c r="A143" s="1" t="s">
         <v>133</v>
       </c>
@@ -13155,7 +13155,7 @@
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8">
       <c r="A144" s="1" t="s">
         <v>132</v>
       </c>
@@ -13171,7 +13171,7 @@
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8">
       <c r="A145" s="1" t="s">
         <v>131</v>
       </c>
@@ -13187,7 +13187,7 @@
       <c r="G145" s="4"/>
       <c r="H145" s="4"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8">
       <c r="A146" s="1" t="s">
         <v>130</v>
       </c>
@@ -13203,7 +13203,7 @@
       <c r="G146" s="4"/>
       <c r="H146" s="4"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8">
       <c r="A147" s="1" t="s">
         <v>129</v>
       </c>
@@ -13219,7 +13219,7 @@
       <c r="G147" s="4"/>
       <c r="H147" s="4"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8">
       <c r="A148" s="1" t="s">
         <v>128</v>
       </c>
@@ -13235,7 +13235,7 @@
       <c r="G148" s="4"/>
       <c r="H148" s="4"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8">
       <c r="A149" s="1" t="s">
         <v>127</v>
       </c>
@@ -13251,7 +13251,7 @@
       <c r="G149" s="4"/>
       <c r="H149" s="4"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8">
       <c r="A150" s="1" t="s">
         <v>126</v>
       </c>
@@ -13267,7 +13267,7 @@
       <c r="G150" s="4"/>
       <c r="H150" s="4"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8">
       <c r="A151" s="1" t="s">
         <v>125</v>
       </c>
@@ -13283,7 +13283,7 @@
       <c r="G151" s="4"/>
       <c r="H151" s="4"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8">
       <c r="A152" s="1" t="s">
         <v>124</v>
       </c>
@@ -13299,7 +13299,7 @@
       <c r="G152" s="4"/>
       <c r="H152" s="4"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8">
       <c r="A153" s="1" t="s">
         <v>123</v>
       </c>
@@ -13315,7 +13315,7 @@
       <c r="G153" s="4"/>
       <c r="H153" s="4"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8">
       <c r="A154" s="1" t="s">
         <v>122</v>
       </c>
@@ -13331,7 +13331,7 @@
       <c r="G154" s="4"/>
       <c r="H154" s="4"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8">
       <c r="A155" s="1" t="s">
         <v>121</v>
       </c>
@@ -13347,7 +13347,7 @@
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8">
       <c r="A156" s="1" t="s">
         <v>120</v>
       </c>
@@ -13363,7 +13363,7 @@
       <c r="G156" s="4"/>
       <c r="H156" s="4"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8">
       <c r="A157" s="1" t="s">
         <v>119</v>
       </c>
@@ -13379,7 +13379,7 @@
       <c r="G157" s="4"/>
       <c r="H157" s="4"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8">
       <c r="A158" s="1" t="s">
         <v>118</v>
       </c>
@@ -13395,7 +13395,7 @@
       <c r="G158" s="4"/>
       <c r="H158" s="4"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8">
       <c r="A159" s="1" t="s">
         <v>117</v>
       </c>
@@ -13411,7 +13411,7 @@
       <c r="G159" s="4"/>
       <c r="H159" s="4"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8">
       <c r="A160" s="1" t="s">
         <v>116</v>
       </c>
@@ -13427,7 +13427,7 @@
       <c r="G160" s="4"/>
       <c r="H160" s="4"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8">
       <c r="A161" s="1" t="s">
         <v>115</v>
       </c>
@@ -13443,7 +13443,7 @@
       <c r="G161" s="4"/>
       <c r="H161" s="4"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8">
       <c r="A162" s="1" t="s">
         <v>114</v>
       </c>
@@ -13459,7 +13459,7 @@
       <c r="G162" s="4"/>
       <c r="H162" s="4"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8">
       <c r="A163" s="1" t="s">
         <v>113</v>
       </c>
@@ -13475,7 +13475,7 @@
       <c r="G163" s="4"/>
       <c r="H163" s="4"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8">
       <c r="A164" s="1" t="s">
         <v>112</v>
       </c>
@@ -13491,7 +13491,7 @@
       <c r="G164" s="4"/>
       <c r="H164" s="4"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8">
       <c r="A165" s="1" t="s">
         <v>111</v>
       </c>
@@ -13507,7 +13507,7 @@
       <c r="G165" s="4"/>
       <c r="H165" s="4"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8">
       <c r="A166" s="1" t="s">
         <v>110</v>
       </c>
@@ -13523,7 +13523,7 @@
       <c r="G166" s="4"/>
       <c r="H166" s="4"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8">
       <c r="A167" s="1" t="s">
         <v>109</v>
       </c>
@@ -13539,7 +13539,7 @@
       <c r="G167" s="4"/>
       <c r="H167" s="4"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8">
       <c r="A168" s="1" t="s">
         <v>108</v>
       </c>
@@ -13555,7 +13555,7 @@
       <c r="G168" s="4"/>
       <c r="H168" s="4"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8">
       <c r="A169" s="1" t="s">
         <v>107</v>
       </c>
@@ -13571,7 +13571,7 @@
       <c r="G169" s="4"/>
       <c r="H169" s="4"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8">
       <c r="A170" s="1" t="s">
         <v>106</v>
       </c>
@@ -13587,7 +13587,7 @@
       <c r="G170" s="4"/>
       <c r="H170" s="4"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8">
       <c r="A171" s="1" t="s">
         <v>105</v>
       </c>
@@ -13603,7 +13603,7 @@
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8">
       <c r="A172" s="1" t="s">
         <v>104</v>
       </c>
@@ -13619,7 +13619,7 @@
       <c r="G172" s="4"/>
       <c r="H172" s="4"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8">
       <c r="A173" s="1" t="s">
         <v>103</v>
       </c>
@@ -13635,7 +13635,7 @@
       <c r="G173" s="4"/>
       <c r="H173" s="4"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8">
       <c r="A174" s="1" t="s">
         <v>102</v>
       </c>
@@ -13651,7 +13651,7 @@
       <c r="G174" s="4"/>
       <c r="H174" s="4"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8">
       <c r="A175" s="1" t="s">
         <v>101</v>
       </c>
@@ -13667,7 +13667,7 @@
       <c r="G175" s="4"/>
       <c r="H175" s="4"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8">
       <c r="A176" s="1" t="s">
         <v>100</v>
       </c>
@@ -13683,7 +13683,7 @@
       <c r="G176" s="4"/>
       <c r="H176" s="4"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8">
       <c r="A177" s="1" t="s">
         <v>99</v>
       </c>
@@ -13699,7 +13699,7 @@
       <c r="G177" s="4"/>
       <c r="H177" s="4"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8">
       <c r="A178" s="1" t="s">
         <v>98</v>
       </c>
@@ -13715,7 +13715,7 @@
       <c r="G178" s="4"/>
       <c r="H178" s="4"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8">
       <c r="A179" s="1" t="s">
         <v>97</v>
       </c>
@@ -13731,7 +13731,7 @@
       <c r="G179" s="4"/>
       <c r="H179" s="4"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8">
       <c r="A180" s="1" t="s">
         <v>96</v>
       </c>
@@ -13747,7 +13747,7 @@
       <c r="G180" s="4"/>
       <c r="H180" s="4"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8">
       <c r="A181" s="1" t="s">
         <v>95</v>
       </c>
@@ -13763,7 +13763,7 @@
       <c r="G181" s="4"/>
       <c r="H181" s="4"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8">
       <c r="A182" s="1" t="s">
         <v>94</v>
       </c>
@@ -13779,7 +13779,7 @@
       <c r="G182" s="4"/>
       <c r="H182" s="4"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8">
       <c r="A183" s="1" t="s">
         <v>93</v>
       </c>
@@ -13795,7 +13795,7 @@
       <c r="G183" s="4"/>
       <c r="H183" s="4"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8">
       <c r="A184" s="1" t="s">
         <v>92</v>
       </c>
@@ -13811,7 +13811,7 @@
       <c r="G184" s="4"/>
       <c r="H184" s="4"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8">
       <c r="A185" s="1" t="s">
         <v>91</v>
       </c>
@@ -13827,7 +13827,7 @@
       <c r="G185" s="4"/>
       <c r="H185" s="4"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8">
       <c r="A186" s="1" t="s">
         <v>90</v>
       </c>
@@ -13843,7 +13843,7 @@
       <c r="G186" s="4"/>
       <c r="H186" s="4"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8">
       <c r="A187" s="1" t="s">
         <v>89</v>
       </c>
@@ -13859,7 +13859,7 @@
       <c r="G187" s="4"/>
       <c r="H187" s="4"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8">
       <c r="A188" s="1" t="s">
         <v>88</v>
       </c>
@@ -13875,7 +13875,7 @@
       <c r="G188" s="4"/>
       <c r="H188" s="4"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8">
       <c r="A189" s="1" t="s">
         <v>87</v>
       </c>
@@ -13891,7 +13891,7 @@
       <c r="G189" s="4"/>
       <c r="H189" s="4"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8">
       <c r="A190" s="1" t="s">
         <v>86</v>
       </c>
@@ -13907,7 +13907,7 @@
       <c r="G190" s="4"/>
       <c r="H190" s="4"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8">
       <c r="A191" s="1" t="s">
         <v>85</v>
       </c>
@@ -13923,7 +13923,7 @@
       <c r="G191" s="4"/>
       <c r="H191" s="4"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8">
       <c r="A192" s="1" t="s">
         <v>84</v>
       </c>
@@ -13939,7 +13939,7 @@
       <c r="G192" s="4"/>
       <c r="H192" s="4"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8">
       <c r="A193" s="1" t="s">
         <v>83</v>
       </c>
@@ -13955,7 +13955,7 @@
       <c r="G193" s="4"/>
       <c r="H193" s="4"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8">
       <c r="A194" s="1" t="s">
         <v>82</v>
       </c>
@@ -13971,7 +13971,7 @@
       <c r="G194" s="4"/>
       <c r="H194" s="4"/>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8">
       <c r="A195" s="1" t="s">
         <v>81</v>
       </c>
@@ -13987,7 +13987,7 @@
       <c r="G195" s="4"/>
       <c r="H195" s="4"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8">
       <c r="A196" s="1" t="s">
         <v>80</v>
       </c>
@@ -14003,7 +14003,7 @@
       <c r="G196" s="4"/>
       <c r="H196" s="4"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8">
       <c r="A197" s="1" t="s">
         <v>79</v>
       </c>
@@ -14019,7 +14019,7 @@
       <c r="G197" s="4"/>
       <c r="H197" s="4"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8">
       <c r="A198" s="1" t="s">
         <v>78</v>
       </c>
@@ -14035,7 +14035,7 @@
       <c r="G198" s="4"/>
       <c r="H198" s="4"/>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8">
       <c r="A199" s="1" t="s">
         <v>77</v>
       </c>
@@ -14051,7 +14051,7 @@
       <c r="G199" s="4"/>
       <c r="H199" s="4"/>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8">
       <c r="A200" s="1" t="s">
         <v>76</v>
       </c>
@@ -14067,7 +14067,7 @@
       <c r="G200" s="4"/>
       <c r="H200" s="4"/>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8">
       <c r="A201" s="1" t="s">
         <v>75</v>
       </c>
@@ -14083,7 +14083,7 @@
       <c r="G201" s="4"/>
       <c r="H201" s="4"/>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8">
       <c r="A202" s="1" t="s">
         <v>74</v>
       </c>
@@ -14099,7 +14099,7 @@
       <c r="G202" s="4"/>
       <c r="H202" s="4"/>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8">
       <c r="A203" s="1" t="s">
         <v>73</v>
       </c>
@@ -14115,7 +14115,7 @@
       <c r="G203" s="4"/>
       <c r="H203" s="4"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8">
       <c r="A204" s="1" t="s">
         <v>72</v>
       </c>
@@ -14131,7 +14131,7 @@
       <c r="G204" s="4"/>
       <c r="H204" s="4"/>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8">
       <c r="A205" s="1" t="s">
         <v>71</v>
       </c>
@@ -14147,7 +14147,7 @@
       <c r="G205" s="4"/>
       <c r="H205" s="4"/>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8">
       <c r="A206" s="1" t="s">
         <v>70</v>
       </c>
@@ -14163,7 +14163,7 @@
       <c r="G206" s="4"/>
       <c r="H206" s="4"/>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8">
       <c r="A207" s="1" t="s">
         <v>69</v>
       </c>
@@ -14179,7 +14179,7 @@
       <c r="G207" s="4"/>
       <c r="H207" s="4"/>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8">
       <c r="A208" s="1" t="s">
         <v>68</v>
       </c>
@@ -14195,7 +14195,7 @@
       <c r="G208" s="4"/>
       <c r="H208" s="4"/>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8">
       <c r="A209" s="1" t="s">
         <v>67</v>
       </c>
@@ -14211,7 +14211,7 @@
       <c r="G209" s="4"/>
       <c r="H209" s="4"/>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8">
       <c r="A210" s="1" t="s">
         <v>66</v>
       </c>
@@ -14227,7 +14227,7 @@
       <c r="G210" s="4"/>
       <c r="H210" s="4"/>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8">
       <c r="A211" s="1" t="s">
         <v>65</v>
       </c>
@@ -14243,7 +14243,7 @@
       <c r="G211" s="4"/>
       <c r="H211" s="4"/>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8">
       <c r="A212" s="1" t="s">
         <v>64</v>
       </c>
@@ -14259,7 +14259,7 @@
       <c r="G212" s="4"/>
       <c r="H212" s="4"/>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8">
       <c r="A213" s="1" t="s">
         <v>63</v>
       </c>
@@ -14275,7 +14275,7 @@
       <c r="G213" s="4"/>
       <c r="H213" s="4"/>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8">
       <c r="A214" s="1" t="s">
         <v>62</v>
       </c>
@@ -14291,7 +14291,7 @@
       <c r="G214" s="4"/>
       <c r="H214" s="4"/>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8">
       <c r="A215" s="1" t="s">
         <v>61</v>
       </c>
@@ -14307,7 +14307,7 @@
       <c r="G215" s="4"/>
       <c r="H215" s="4"/>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8">
       <c r="A216" s="1" t="s">
         <v>60</v>
       </c>
@@ -14323,7 +14323,7 @@
       <c r="G216" s="4"/>
       <c r="H216" s="4"/>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8">
       <c r="A217" s="1" t="s">
         <v>59</v>
       </c>
@@ -14339,7 +14339,7 @@
       <c r="G217" s="4"/>
       <c r="H217" s="4"/>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8">
       <c r="A218" s="1" t="s">
         <v>58</v>
       </c>
@@ -14355,7 +14355,7 @@
       <c r="G218" s="4"/>
       <c r="H218" s="4"/>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8">
       <c r="A219" s="1" t="s">
         <v>57</v>
       </c>
@@ -14371,7 +14371,7 @@
       <c r="G219" s="4"/>
       <c r="H219" s="4"/>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8">
       <c r="A220" s="1" t="s">
         <v>56</v>
       </c>
@@ -14387,7 +14387,7 @@
       <c r="G220" s="4"/>
       <c r="H220" s="4"/>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:8">
       <c r="A221" s="1" t="s">
         <v>55</v>
       </c>
@@ -14403,7 +14403,7 @@
       <c r="G221" s="4"/>
       <c r="H221" s="4"/>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:8">
       <c r="A222" s="1" t="s">
         <v>54</v>
       </c>
@@ -14419,7 +14419,7 @@
       <c r="G222" s="4"/>
       <c r="H222" s="4"/>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:8">
       <c r="A223" s="1" t="s">
         <v>53</v>
       </c>
@@ -14435,7 +14435,7 @@
       <c r="G223" s="4"/>
       <c r="H223" s="4"/>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:8">
       <c r="A224" s="5" t="s">
         <v>52</v>
       </c>
@@ -14451,7 +14451,7 @@
       <c r="G224" s="4"/>
       <c r="H224" s="4"/>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8">
       <c r="A225" s="5" t="s">
         <v>51</v>
       </c>
@@ -14467,7 +14467,7 @@
       <c r="G225" s="4"/>
       <c r="H225" s="4"/>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8">
       <c r="A226" s="5" t="s">
         <v>50</v>
       </c>
@@ -14483,7 +14483,7 @@
       <c r="G226" s="4"/>
       <c r="H226" s="4"/>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8">
       <c r="A227" s="5" t="s">
         <v>49</v>
       </c>
@@ -14499,7 +14499,7 @@
       <c r="G227" s="4"/>
       <c r="H227" s="4"/>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8">
       <c r="A228" s="5" t="s">
         <v>48</v>
       </c>
@@ -14515,7 +14515,7 @@
       <c r="G228" s="4"/>
       <c r="H228" s="4"/>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8">
       <c r="A229" s="5" t="s">
         <v>47</v>
       </c>
@@ -14531,7 +14531,7 @@
       <c r="G229" s="4"/>
       <c r="H229" s="4"/>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8">
       <c r="A230" s="5" t="s">
         <v>46</v>
       </c>
@@ -14547,7 +14547,7 @@
       <c r="G230" s="4"/>
       <c r="H230" s="4"/>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8">
       <c r="A231" s="6" t="s">
         <v>45</v>
       </c>
@@ -14563,7 +14563,7 @@
       <c r="G231" s="4"/>
       <c r="H231" s="4"/>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8">
       <c r="A232" s="6" t="s">
         <v>44</v>
       </c>
@@ -14579,7 +14579,7 @@
       <c r="G232" s="4"/>
       <c r="H232" s="4"/>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8">
       <c r="A233" s="6" t="s">
         <v>43</v>
       </c>
@@ -14595,7 +14595,7 @@
       <c r="G233" s="4"/>
       <c r="H233" s="4"/>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8">
       <c r="A234" s="6" t="s">
         <v>42</v>
       </c>
@@ -14611,7 +14611,7 @@
       <c r="G234" s="4"/>
       <c r="H234" s="4"/>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8">
       <c r="A235" s="6" t="s">
         <v>41</v>
       </c>
@@ -14627,7 +14627,7 @@
       <c r="G235" s="4"/>
       <c r="H235" s="4"/>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8">
       <c r="A236" s="6" t="s">
         <v>40</v>
       </c>
@@ -14643,7 +14643,7 @@
       <c r="G236" s="4"/>
       <c r="H236" s="4"/>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8">
       <c r="A237" s="6" t="s">
         <v>39</v>
       </c>
@@ -14657,7 +14657,7 @@
       <c r="E237" s="3"/>
       <c r="F237" s="3"/>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8">
       <c r="A238" s="6" t="s">
         <v>38</v>
       </c>
@@ -14671,7 +14671,7 @@
       <c r="E238" s="3"/>
       <c r="F238" s="3"/>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8">
       <c r="A239" s="6" t="s">
         <v>37</v>
       </c>
@@ -14685,7 +14685,7 @@
       <c r="E239" s="3"/>
       <c r="F239" s="3"/>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8">
       <c r="A240" s="6" t="s">
         <v>36</v>
       </c>
@@ -14699,7 +14699,7 @@
       <c r="E240" s="3"/>
       <c r="F240" s="3"/>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:6">
       <c r="A241" s="6" t="s">
         <v>35</v>
       </c>
@@ -14713,7 +14713,7 @@
       <c r="E241" s="3"/>
       <c r="F241" s="3"/>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6">
       <c r="A242" s="6" t="s">
         <v>34</v>
       </c>
@@ -14727,7 +14727,7 @@
       <c r="E242" s="3"/>
       <c r="F242" s="3"/>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:6">
       <c r="A243" s="6" t="s">
         <v>33</v>
       </c>
@@ -14741,7 +14741,7 @@
       <c r="E243" s="3"/>
       <c r="F243" s="3"/>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6">
       <c r="A244" s="6" t="s">
         <v>32</v>
       </c>
@@ -14755,7 +14755,7 @@
       <c r="E244" s="3"/>
       <c r="F244" s="3"/>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:6">
       <c r="A245" s="6" t="s">
         <v>31</v>
       </c>
@@ -14769,7 +14769,7 @@
       <c r="E245" s="3"/>
       <c r="F245" s="3"/>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6">
       <c r="A246" s="6" t="s">
         <v>30</v>
       </c>
@@ -14783,7 +14783,7 @@
       <c r="E246" s="3"/>
       <c r="F246" s="3"/>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:6">
       <c r="A247" s="6" t="s">
         <v>29</v>
       </c>
@@ -14797,7 +14797,7 @@
       <c r="E247" s="3"/>
       <c r="F247" s="3"/>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:6">
       <c r="A248" s="6" t="s">
         <v>28</v>
       </c>
@@ -14811,7 +14811,7 @@
       <c r="E248" s="3"/>
       <c r="F248" s="3"/>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:6">
       <c r="A249" s="6" t="s">
         <v>27</v>
       </c>
@@ -14825,7 +14825,7 @@
       <c r="E249" s="3"/>
       <c r="F249" s="3"/>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:6">
       <c r="A250" s="6" t="s">
         <v>26</v>
       </c>
@@ -14839,7 +14839,7 @@
       <c r="E250" s="3"/>
       <c r="F250" s="3"/>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6">
       <c r="A251" s="6" t="s">
         <v>25</v>
       </c>
@@ -14853,7 +14853,7 @@
       <c r="E251" s="3"/>
       <c r="F251" s="3"/>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:6">
       <c r="A252" s="6" t="s">
         <v>24</v>
       </c>
@@ -14867,7 +14867,7 @@
       <c r="E252" s="3"/>
       <c r="F252" s="3"/>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6">
       <c r="A253" s="6" t="s">
         <v>23</v>
       </c>
@@ -14881,7 +14881,7 @@
       <c r="E253" s="3"/>
       <c r="F253" s="3"/>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6">
       <c r="A254" s="6" t="s">
         <v>22</v>
       </c>
@@ -14895,7 +14895,7 @@
       <c r="E254" s="3"/>
       <c r="F254" s="3"/>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:6">
       <c r="A255" s="6" t="s">
         <v>21</v>
       </c>
@@ -14909,7 +14909,7 @@
       <c r="E255" s="3"/>
       <c r="F255" s="3"/>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:6">
       <c r="A256" s="6" t="s">
         <v>20</v>
       </c>
@@ -14923,7 +14923,7 @@
       <c r="E256" s="3"/>
       <c r="F256" s="3"/>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6">
       <c r="A257" s="6" t="s">
         <v>19</v>
       </c>
@@ -14937,7 +14937,7 @@
       <c r="E257" s="3"/>
       <c r="F257" s="3"/>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6">
       <c r="A258" s="6" t="s">
         <v>18</v>
       </c>
@@ -14951,7 +14951,7 @@
       <c r="E258" s="3"/>
       <c r="F258" s="3"/>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6">
       <c r="A259" s="6" t="s">
         <v>17</v>
       </c>
@@ -14965,7 +14965,7 @@
       <c r="E259" s="3"/>
       <c r="F259" s="3"/>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6">
       <c r="A260" s="6" t="s">
         <v>16</v>
       </c>
@@ -14979,7 +14979,7 @@
       <c r="E260" s="3"/>
       <c r="F260" s="3"/>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6">
       <c r="A261" s="6" t="s">
         <v>15</v>
       </c>
@@ -14993,7 +14993,7 @@
       <c r="E261" s="3"/>
       <c r="F261" s="3"/>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:6">
       <c r="A262" s="6" t="s">
         <v>14</v>
       </c>
@@ -15007,7 +15007,7 @@
       <c r="E262" s="3"/>
       <c r="F262" s="3"/>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:6">
       <c r="A263" s="6" t="s">
         <v>13</v>
       </c>
@@ -15021,7 +15021,7 @@
       <c r="E263" s="3"/>
       <c r="F263" s="3"/>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:6">
       <c r="A264" s="6" t="s">
         <v>12</v>
       </c>
@@ -15035,7 +15035,7 @@
       <c r="E264" s="3"/>
       <c r="F264" s="3"/>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:6">
       <c r="A265" s="6" t="s">
         <v>11</v>
       </c>
@@ -15049,7 +15049,7 @@
       <c r="E265" s="3"/>
       <c r="F265" s="3"/>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:6">
       <c r="A266" s="6" t="s">
         <v>10</v>
       </c>
@@ -15063,7 +15063,7 @@
       <c r="E266" s="3"/>
       <c r="F266" s="3"/>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:6">
       <c r="A267" s="6" t="s">
         <v>9</v>
       </c>
@@ -15077,7 +15077,7 @@
       <c r="E267" s="3"/>
       <c r="F267" s="3"/>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:6">
       <c r="A268" s="6" t="s">
         <v>8</v>
       </c>
@@ -15091,7 +15091,7 @@
       <c r="E268" s="3"/>
       <c r="F268" s="3"/>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:6">
       <c r="A269" s="6" t="s">
         <v>7</v>
       </c>
@@ -15105,7 +15105,7 @@
       <c r="E269" s="3"/>
       <c r="F269" s="3"/>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:6">
       <c r="A270" s="6" t="s">
         <v>6</v>
       </c>
@@ -15119,7 +15119,7 @@
       <c r="E270" s="3"/>
       <c r="F270" s="3"/>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:6">
       <c r="A271" s="6" t="s">
         <v>5</v>
       </c>
@@ -15133,7 +15133,7 @@
       <c r="E271" s="3"/>
       <c r="F271" s="3"/>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:6">
       <c r="A272" s="6" t="s">
         <v>4</v>
       </c>
@@ -15147,7 +15147,7 @@
       <c r="E272" s="3"/>
       <c r="F272" s="3"/>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:6">
       <c r="A273" s="6" t="s">
         <v>3</v>
       </c>
@@ -15161,7 +15161,7 @@
       <c r="E273" s="3"/>
       <c r="F273" s="3"/>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:6">
       <c r="A274" s="6" t="s">
         <v>2</v>
       </c>
@@ -15175,7 +15175,7 @@
       <c r="E274" s="3"/>
       <c r="F274" s="3"/>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:6">
       <c r="A275" s="6" t="s">
         <v>1</v>
       </c>
@@ -15189,7 +15189,7 @@
       <c r="E275" s="3"/>
       <c r="F275" s="3"/>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:6">
       <c r="A276" s="6" t="s">
         <v>0</v>
       </c>
@@ -15203,7 +15203,7 @@
       <c r="E276" s="3"/>
       <c r="F276" s="3"/>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:6">
       <c r="A277" s="6" t="s">
         <v>277</v>
       </c>
@@ -15217,7 +15217,7 @@
       <c r="E277" s="3"/>
       <c r="F277" s="3"/>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:6">
       <c r="A278" s="6" t="s">
         <v>278</v>
       </c>
@@ -15231,7 +15231,7 @@
       <c r="E278" s="3"/>
       <c r="F278" s="3"/>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:6">
       <c r="A279" s="6" t="s">
         <v>279</v>
       </c>
@@ -15245,7 +15245,7 @@
       <c r="E279" s="3"/>
       <c r="F279" s="3"/>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:6">
       <c r="A280" s="6" t="s">
         <v>280</v>
       </c>
@@ -15259,7 +15259,7 @@
       <c r="E280" s="3"/>
       <c r="F280" s="3"/>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:6">
       <c r="A281" s="6" t="s">
         <v>281</v>
       </c>
@@ -15273,7 +15273,7 @@
       <c r="E281" s="3"/>
       <c r="F281" s="3"/>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:6">
       <c r="A282" s="6" t="s">
         <v>282</v>
       </c>
@@ -15287,7 +15287,7 @@
       <c r="E282" s="3"/>
       <c r="F282" s="3"/>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:6">
       <c r="A283" s="6" t="s">
         <v>283</v>
       </c>
@@ -15301,7 +15301,7 @@
       <c r="E283" s="3"/>
       <c r="F283" s="3"/>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:6">
       <c r="A284" s="6" t="s">
         <v>284</v>
       </c>
@@ -15315,7 +15315,7 @@
       <c r="E284" s="3"/>
       <c r="F284" s="3"/>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:6">
       <c r="A285" s="6" t="s">
         <v>285</v>
       </c>
@@ -15329,7 +15329,7 @@
       <c r="E285" s="3"/>
       <c r="F285" s="3"/>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:6">
       <c r="A286" s="6" t="s">
         <v>286</v>
       </c>
@@ -15343,7 +15343,7 @@
       <c r="E286" s="3"/>
       <c r="F286" s="3"/>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:6">
       <c r="A287" s="6" t="s">
         <v>287</v>
       </c>
@@ -15357,7 +15357,7 @@
       <c r="E287" s="3"/>
       <c r="F287" s="3"/>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:6">
       <c r="A288" s="6" t="s">
         <v>288</v>
       </c>
@@ -15371,7 +15371,7 @@
       <c r="E288" s="3"/>
       <c r="F288" s="3"/>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:6">
       <c r="A289" s="6" t="s">
         <v>289</v>
       </c>
@@ -15385,7 +15385,7 @@
       <c r="E289" s="3"/>
       <c r="F289" s="3"/>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:6">
       <c r="A290" s="6" t="s">
         <v>290</v>
       </c>
@@ -15399,7 +15399,7 @@
       <c r="E290" s="3"/>
       <c r="F290" s="3"/>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:6">
       <c r="A291" s="6" t="s">
         <v>291</v>
       </c>
@@ -15413,7 +15413,7 @@
       <c r="E291" s="3"/>
       <c r="F291" s="3"/>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:6">
       <c r="A292" s="6" t="s">
         <v>292</v>
       </c>
@@ -15427,7 +15427,7 @@
       <c r="E292" s="3"/>
       <c r="F292" s="3"/>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:6">
       <c r="A293" s="6" t="s">
         <v>293</v>
       </c>
@@ -15441,7 +15441,7 @@
       <c r="E293" s="3"/>
       <c r="F293" s="3"/>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:6">
       <c r="A294" s="6" t="s">
         <v>294</v>
       </c>
@@ -15455,7 +15455,7 @@
       <c r="E294" s="3"/>
       <c r="F294" s="3"/>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:6">
       <c r="A295" s="6" t="s">
         <v>295</v>
       </c>
@@ -15469,7 +15469,7 @@
       <c r="E295" s="3"/>
       <c r="F295" s="3"/>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:6">
       <c r="A296" s="6" t="s">
         <v>296</v>
       </c>
@@ -15483,7 +15483,7 @@
       <c r="E296" s="3"/>
       <c r="F296" s="3"/>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:6">
       <c r="A297" s="6" t="s">
         <v>297</v>
       </c>
@@ -15497,7 +15497,7 @@
       <c r="E297" s="3"/>
       <c r="F297" s="3"/>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:6">
       <c r="A298" s="6" t="s">
         <v>298</v>
       </c>
@@ -15511,7 +15511,7 @@
       <c r="E298" s="3"/>
       <c r="F298" s="3"/>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:6">
       <c r="A299" s="6" t="s">
         <v>299</v>
       </c>
@@ -15525,7 +15525,7 @@
       <c r="E299" s="3"/>
       <c r="F299" s="3"/>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:6">
       <c r="A300" s="6" t="s">
         <v>300</v>
       </c>
@@ -15539,7 +15539,7 @@
       <c r="E300" s="3"/>
       <c r="F300" s="3"/>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:6">
       <c r="A301" s="6" t="s">
         <v>301</v>
       </c>
@@ -15553,7 +15553,7 @@
       <c r="E301" s="3"/>
       <c r="F301" s="3"/>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:6">
       <c r="A302" s="6" t="s">
         <v>302</v>
       </c>
@@ -15567,7 +15567,7 @@
       <c r="E302" s="3"/>
       <c r="F302" s="3"/>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:6">
       <c r="A303" s="6" t="s">
         <v>303</v>
       </c>
@@ -15581,7 +15581,7 @@
       <c r="E303" s="3"/>
       <c r="F303" s="3"/>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:6">
       <c r="A304" s="6" t="s">
         <v>304</v>
       </c>
@@ -15595,7 +15595,7 @@
       <c r="E304" s="3"/>
       <c r="F304" s="3"/>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:6">
       <c r="A305" s="6" t="s">
         <v>305</v>
       </c>
@@ -15609,7 +15609,7 @@
       <c r="E305" s="3"/>
       <c r="F305" s="3"/>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:6">
       <c r="A306" s="6" t="s">
         <v>306</v>
       </c>
@@ -15623,7 +15623,7 @@
       <c r="E306" s="3"/>
       <c r="F306" s="3"/>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:6">
       <c r="A307" s="6" t="s">
         <v>307</v>
       </c>
@@ -15637,7 +15637,7 @@
       <c r="E307" s="3"/>
       <c r="F307" s="3"/>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:6">
       <c r="A308" s="6" t="s">
         <v>308</v>
       </c>
@@ -15651,7 +15651,7 @@
       <c r="E308" s="3"/>
       <c r="F308" s="3"/>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:6">
       <c r="A309" s="6" t="s">
         <v>309</v>
       </c>
@@ -15665,7 +15665,7 @@
       <c r="E309" s="3"/>
       <c r="F309" s="3"/>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:6">
       <c r="A310" s="6" t="s">
         <v>310</v>
       </c>
@@ -15679,7 +15679,7 @@
       <c r="E310" s="3"/>
       <c r="F310" s="3"/>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:6">
       <c r="A311" s="6" t="s">
         <v>311</v>
       </c>
@@ -15693,7 +15693,7 @@
       <c r="E311" s="3"/>
       <c r="F311" s="3"/>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:6">
       <c r="A312" s="6" t="s">
         <v>312</v>
       </c>
@@ -15707,7 +15707,7 @@
       <c r="E312" s="3"/>
       <c r="F312" s="3"/>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:6">
       <c r="A313" s="6" t="s">
         <v>313</v>
       </c>
@@ -15721,7 +15721,7 @@
       <c r="E313" s="3"/>
       <c r="F313" s="3"/>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:6">
       <c r="A314" s="6" t="s">
         <v>314</v>
       </c>
@@ -15734,7 +15734,7 @@
       <c r="E314" s="3"/>
       <c r="F314" s="3"/>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:6">
       <c r="A315" s="6" t="s">
         <v>315</v>
       </c>
@@ -15747,7 +15747,7 @@
       <c r="E315" s="3"/>
       <c r="F315" s="3"/>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:6">
       <c r="A316" s="6" t="s">
         <v>316</v>
       </c>
@@ -15760,7 +15760,7 @@
       <c r="E316" s="3"/>
       <c r="F316" s="3"/>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:6">
       <c r="A317" s="6" t="s">
         <v>317</v>
       </c>
@@ -15773,7 +15773,7 @@
       <c r="E317" s="3"/>
       <c r="F317" s="3"/>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:6">
       <c r="A318" s="6" t="s">
         <v>318</v>
       </c>
@@ -15786,7 +15786,7 @@
       <c r="E318" s="3"/>
       <c r="F318" s="3"/>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:6">
       <c r="A319" s="6" t="s">
         <v>319</v>
       </c>
@@ -15799,7 +15799,7 @@
       <c r="E319" s="3"/>
       <c r="F319" s="3"/>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:6">
       <c r="A320" s="6" t="s">
         <v>324</v>
       </c>
@@ -15812,7 +15812,7 @@
       <c r="E320" s="3"/>
       <c r="F320" s="3"/>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:6">
       <c r="A321" s="6" t="s">
         <v>325</v>
       </c>
@@ -15825,7 +15825,7 @@
       <c r="E321" s="3"/>
       <c r="F321" s="3"/>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:6">
       <c r="A322" s="6" t="s">
         <v>326</v>
       </c>
@@ -15838,7 +15838,7 @@
       <c r="E322" s="3"/>
       <c r="F322" s="3"/>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:6">
       <c r="A323" s="6" t="s">
         <v>327</v>
       </c>
@@ -15851,7 +15851,7 @@
       <c r="E323" s="3"/>
       <c r="F323" s="3"/>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:6">
       <c r="A324" s="6" t="s">
         <v>328</v>
       </c>
@@ -15864,7 +15864,7 @@
       <c r="E324" s="3"/>
       <c r="F324" s="3"/>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:6">
       <c r="A325" s="6" t="s">
         <v>329</v>
       </c>
@@ -15877,7 +15877,7 @@
       <c r="E325" s="3"/>
       <c r="F325" s="3"/>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:6">
       <c r="A326" s="6" t="s">
         <v>330</v>
       </c>
@@ -15890,7 +15890,7 @@
       <c r="E326" s="3"/>
       <c r="F326" s="3"/>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:6">
       <c r="A327" s="6" t="s">
         <v>331</v>
       </c>
@@ -15903,7 +15903,7 @@
       <c r="E327" s="3"/>
       <c r="F327" s="3"/>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:6">
       <c r="A328" s="6" t="s">
         <v>332</v>
       </c>
@@ -15916,7 +15916,7 @@
       <c r="E328" s="3"/>
       <c r="F328" s="3"/>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:6">
       <c r="A329" s="6" t="s">
         <v>333</v>
       </c>
@@ -15929,7 +15929,7 @@
       <c r="E329" s="3"/>
       <c r="F329" s="3"/>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:6">
       <c r="A330" s="6" t="s">
         <v>334</v>
       </c>
@@ -15942,7 +15942,7 @@
       <c r="E330" s="3"/>
       <c r="F330" s="3"/>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:6">
       <c r="A331" s="6" t="s">
         <v>335</v>
       </c>
@@ -15955,7 +15955,7 @@
       <c r="E331" s="3"/>
       <c r="F331" s="3"/>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:6">
       <c r="A332" s="6" t="s">
         <v>336</v>
       </c>
@@ -15968,7 +15968,7 @@
       <c r="E332" s="3"/>
       <c r="F332" s="3"/>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:6">
       <c r="A333" s="6" t="s">
         <v>337</v>
       </c>
@@ -15981,7 +15981,7 @@
       <c r="E333" s="3"/>
       <c r="F333" s="3"/>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:6">
       <c r="A334" s="6" t="s">
         <v>338</v>
       </c>
@@ -15994,7 +15994,7 @@
       <c r="E334" s="3"/>
       <c r="F334" s="3"/>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:6">
       <c r="A335" s="6" t="s">
         <v>340</v>
       </c>
@@ -16007,7 +16007,7 @@
       <c r="E335" s="3"/>
       <c r="F335" s="3"/>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:6">
       <c r="A336" s="6" t="s">
         <v>343</v>
       </c>
@@ -16020,7 +16020,7 @@
       <c r="E336" s="3"/>
       <c r="F336" s="3"/>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:6">
       <c r="A337" s="6" t="s">
         <v>348</v>
       </c>
@@ -16033,7 +16033,7 @@
       <c r="E337" s="3"/>
       <c r="F337" s="3"/>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:6">
       <c r="A338" s="6" t="s">
         <v>361</v>
       </c>
@@ -16046,7 +16046,7 @@
       <c r="E338" s="3"/>
       <c r="F338" s="3"/>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:6">
       <c r="A339" s="6" t="s">
         <v>363</v>
       </c>
@@ -16059,7 +16059,7 @@
       <c r="E339" s="3"/>
       <c r="F339" s="3"/>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:6">
       <c r="A340" s="6" t="s">
         <v>366</v>
       </c>
@@ -16071,7 +16071,7 @@
       </c>
       <c r="F340" s="3"/>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:6">
       <c r="A341" s="6" t="s">
         <v>368</v>
       </c>
@@ -16083,7 +16083,7 @@
       </c>
       <c r="F341" s="3"/>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:6">
       <c r="A342" s="6" t="s">
         <v>369</v>
       </c>
@@ -16095,7 +16095,7 @@
       </c>
       <c r="F342" s="3"/>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:6">
       <c r="A343" s="6" t="s">
         <v>372</v>
       </c>
@@ -16108,7 +16108,7 @@
       <c r="E343" s="3"/>
       <c r="F343" s="3"/>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:6">
       <c r="A344" s="6" t="s">
         <v>374</v>
       </c>
@@ -16121,7 +16121,7 @@
       <c r="E344" s="3"/>
       <c r="F344" s="3"/>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:6">
       <c r="A345" s="6" t="s">
         <v>376</v>
       </c>
@@ -16134,7 +16134,7 @@
       <c r="E345" s="3"/>
       <c r="F345" s="3"/>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:6">
       <c r="A346" s="6" t="s">
         <v>379</v>
       </c>
@@ -16147,7 +16147,7 @@
       <c r="E346" s="3"/>
       <c r="F346" s="3"/>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:6">
       <c r="A347" s="6"/>
       <c r="B347" s="3"/>
       <c r="C347" s="3"/>

</xml_diff>